<commit_message>
added new Japan Osaka Schedule
</commit_message>
<xml_diff>
--- a/Time Table Dec 2018.xlsx
+++ b/Time Table Dec 2018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Time</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>วันหยุด</t>
-  </si>
-  <si>
-    <t>ช่วง Osaka …</t>
   </si>
 </sst>
 </file>
@@ -15238,26 +15235,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>424544</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>261256</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="254" name="สี่เหลี่ยมผืนผ้า 253"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14369144" y="12065726"/>
-          <a:ext cx="1828798" cy="419100"/>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>217715</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>119744</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>16329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="259" name="สี่เหลี่ยมผืนผ้า 258"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6193972" y="25037143"/>
+          <a:ext cx="1894115" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15290,12 +15287,8 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Check</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> in in DMK Airport  (Passport + E-Ticket) </a:t>
+            <a:t>Print Boarding Pass</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -15305,25 +15298,167 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>413658</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>293913</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>386443</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="255" name="สี่เหลี่ยมผืนผ้า 254"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9089570" y="12017829"/>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>642257</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>544287</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>419101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="260" name="สี่เหลี่ยมผืนผ้า 259"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5954486" y="18745201"/>
+          <a:ext cx="1894115" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>เตรียมแผนที่ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>osaka, print, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>ที่อยู่โรงแรม</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>206828</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>397329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="261" name="สี่เหลี่ยมผืนผ้า 260"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6183085" y="25864458"/>
+          <a:ext cx="1894115" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>แลกเงิน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>Yen 10000 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>บาท</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>108858</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>402772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>375557</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="262" name="สี่เหลี่ยมผืนผ้า 261"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6085115" y="21379543"/>
           <a:ext cx="1828800" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15355,20 +15490,12 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เตรียมของ ใช้ </a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Ritual </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>พิเศษ สำหรับ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Trip</a:t>
+            <a:t>Policy</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> of Japan Osaka,  read it</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -15668,8 +15795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16619,11 +16746,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J30" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    <row r="30" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43435</v>

</xml_diff>